<commit_message>
formulas for vertical bands
</commit_message>
<xml_diff>
--- a/core/test/smoketest/test1.xlsx
+++ b/core/test/smoketest/test1.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <f>SUM(B3:C3)</f>
+        <f>SUM(E1:E1)</f>
         <v>0</v>
       </c>
       <c r="E3" s="5"/>

</xml_diff>